<commit_message>
Updated for Iteration 2
</commit_message>
<xml_diff>
--- a/Bug Tracking/Bug Tracking System.xlsx
+++ b/Bug Tracking/Bug Tracking System.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Defects</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Employee Asign to project bug</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -82,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -90,26 +93,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -415,17 +443,17 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -434,105 +462,116 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="5">
         <v>41554</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
         <v>0.5</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="6">
         <v>0.25</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="5">
         <v>41554</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="5">
         <v>41572</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>0.5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="8">
         <v>0.5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="9">
         <v>41572</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="5">
         <v>41572</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>0.5</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="8">
         <v>0.5</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="9">
         <v>41572</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="1"/>
+      <c r="C6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="11">
+        <f>SUM(D3:D5)</f>
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="11">
+        <f>SUM(E3:E5)</f>
+        <v>1.25</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor Fixes and DB update
</commit_message>
<xml_diff>
--- a/Bug Tracking/Bug Tracking System.xlsx
+++ b/Bug Tracking/Bug Tracking System.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Defects</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>Sprint initial story points not recording correctly</t>
+  </si>
+  <si>
+    <t>jose</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Name Not changing on all files.  CompanyProperties business name should be on all headers not hard coded beter software</t>
+  </si>
+  <si>
+    <t>Remove Project list slider. Not used effectivly no longer makes sense.</t>
   </si>
 </sst>
 </file>
@@ -446,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,44 +586,94 @@
       <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="D7" s="8">
         <v>0.5</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="C8" s="10" t="s">
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>41604</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>41604</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="C12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D12" s="11">
         <f>SUM(D3:D5)</f>
         <v>1.5</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E12" s="11">
         <f>SUM(E3:E6)</f>
         <v>1.75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>